<commit_message>
working on getting lat long data
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/25_04-08_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/25_04-08_pd_samples-edited.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AE81D2-D033-4F4F-A479-CBB970D6F507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2211370-0E53-7945-B92C-A657A3FBF024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1080" windowWidth="22560" windowHeight="18980" xr2:uid="{6FFE1609-E92B-F149-91DD-BB05A0A86C69}"/>
+    <workbookView xWindow="1500" yWindow="1120" windowWidth="12020" windowHeight="18980" activeTab="1" xr2:uid="{6FFE1609-E92B-F149-91DD-BB05A0A86C69}"/>
   </bookViews>
   <sheets>
-    <sheet name="pd_samples" sheetId="1" r:id="rId1"/>
+    <sheet name="all_pd_samples" sheetId="1" r:id="rId1"/>
+    <sheet name="vcf_pd_samples" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="363">
   <si>
     <t>sample_id</t>
   </si>
@@ -1097,6 +1098,18 @@
   </si>
   <si>
     <t>double check lat long data</t>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>N_America</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1443,6 +1456,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1608,10 +1633,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1994,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671BC494-C93E-4D44-90B8-1DAAA520466A}">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2049,11 +2074,11 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>345</v>
       </c>
       <c r="C2" t="s">
@@ -2077,8 +2102,8 @@
       <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
       <c r="M2" t="s">
         <v>343</v>
       </c>
@@ -2087,7 +2112,7 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>346</v>
       </c>
       <c r="C3" t="s">
@@ -2111,14 +2136,14 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>347</v>
       </c>
       <c r="C4" t="s">
@@ -2142,10 +2167,10 @@
       <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>49.954439999999998</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <v>14.175829999999999</v>
       </c>
       <c r="M4" t="s">
@@ -2156,7 +2181,7 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>348</v>
       </c>
       <c r="C5" t="s">
@@ -2180,10 +2205,10 @@
       <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="4">
         <v>49.954439999999998</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>14.175829999999999</v>
       </c>
       <c r="M5" t="s">
@@ -2194,7 +2219,7 @@
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>349</v>
       </c>
       <c r="C6" t="s">
@@ -2218,10 +2243,10 @@
       <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="4">
         <v>50.693460000000002</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <v>15.84652</v>
       </c>
       <c r="M6" t="s">
@@ -2232,7 +2257,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>350</v>
       </c>
       <c r="C7" t="s">
@@ -2256,10 +2281,10 @@
       <c r="I7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="4">
         <v>50.693460000000002</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="4">
         <v>15.84652</v>
       </c>
       <c r="M7" t="s">
@@ -2270,7 +2295,7 @@
       <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>351</v>
       </c>
       <c r="C8" t="s">
@@ -2291,17 +2316,17 @@
       <c r="H8" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>352</v>
       </c>
       <c r="C9" t="s">
@@ -2322,17 +2347,17 @@
       <c r="H9" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>353</v>
       </c>
       <c r="C10" t="s">
@@ -2353,17 +2378,17 @@
       <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C11" t="s">
@@ -2384,17 +2409,17 @@
       <c r="H11" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C12" t="s">
@@ -2415,17 +2440,17 @@
       <c r="H12" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C13" t="s">
@@ -2446,17 +2471,17 @@
       <c r="H13" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C14" t="s">
@@ -2477,17 +2502,17 @@
       <c r="H14" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C15" t="s">
@@ -2508,17 +2533,17 @@
       <c r="H15" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C16" t="s">
@@ -2539,17 +2564,17 @@
       <c r="H16" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C17" t="s">
@@ -2570,17 +2595,17 @@
       <c r="H17" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C18" t="s">
@@ -2601,17 +2626,17 @@
       <c r="H18" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C19" t="s">
@@ -2632,17 +2657,17 @@
       <c r="H19" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C20" t="s">
@@ -2663,17 +2688,17 @@
       <c r="H20" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>84</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C21" t="s">
@@ -2694,17 +2719,17 @@
       <c r="H21" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C22" t="s">
@@ -2725,17 +2750,17 @@
       <c r="H22" t="s">
         <v>36</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>92</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C23" t="s">
@@ -2756,17 +2781,17 @@
       <c r="H23" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C24" t="s">
@@ -2787,17 +2812,17 @@
       <c r="H24" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>100</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C25" t="s">
@@ -2818,17 +2843,17 @@
       <c r="H25" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>104</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C26" t="s">
@@ -2852,14 +2877,14 @@
       <c r="I26" t="s">
         <v>109</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>110</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C27" t="s">
@@ -2883,14 +2908,14 @@
       <c r="I27" t="s">
         <v>114</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>115</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C28" t="s">
@@ -2914,14 +2939,14 @@
       <c r="I28" t="s">
         <v>119</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>120</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C29" t="s">
@@ -2945,14 +2970,14 @@
       <c r="I29" t="s">
         <v>124</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>125</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C30" t="s">
@@ -2976,14 +3001,14 @@
       <c r="I30" t="s">
         <v>130</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>131</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>132</v>
       </c>
       <c r="C31" t="s">
@@ -3007,14 +3032,14 @@
       <c r="I31" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>136</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C32" t="s">
@@ -3038,14 +3063,14 @@
       <c r="I32" t="s">
         <v>140</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>141</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C33" t="s">
@@ -3069,14 +3094,14 @@
       <c r="I33" t="s">
         <v>145</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C34" t="s">
@@ -3100,14 +3125,14 @@
       <c r="I34" t="s">
         <v>150</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>151</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>152</v>
       </c>
       <c r="C35" t="s">
@@ -3131,14 +3156,14 @@
       <c r="I35" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>125</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C36" t="s">
@@ -3162,14 +3187,14 @@
       <c r="I36" t="s">
         <v>130</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>158</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>159</v>
       </c>
       <c r="C37" t="s">
@@ -3190,15 +3215,15 @@
       <c r="H37" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>158</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C38" t="s">
@@ -3219,15 +3244,15 @@
       <c r="H38" t="s">
         <v>14</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="6" t="s">
         <v>166</v>
       </c>
       <c r="C39" t="s">
@@ -3248,15 +3273,15 @@
       <c r="H39" t="s">
         <v>14</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>169</v>
       </c>
       <c r="C40" t="s">
@@ -3277,15 +3302,15 @@
       <c r="H40" t="s">
         <v>36</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>172</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>173</v>
       </c>
       <c r="C41" t="s">
@@ -3306,15 +3331,15 @@
       <c r="H41" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>172</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="6" t="s">
         <v>176</v>
       </c>
       <c r="C42" t="s">
@@ -3335,15 +3360,15 @@
       <c r="H42" t="s">
         <v>36</v>
       </c>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="6" t="s">
         <v>179</v>
       </c>
       <c r="C43" t="s">
@@ -3364,15 +3389,15 @@
       <c r="H43" t="s">
         <v>36</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>158</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C44" t="s">
@@ -3393,15 +3418,15 @@
       <c r="H44" t="s">
         <v>14</v>
       </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>158</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="6" t="s">
         <v>185</v>
       </c>
       <c r="C45" t="s">
@@ -3422,15 +3447,15 @@
       <c r="H45" t="s">
         <v>14</v>
       </c>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>158</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>188</v>
       </c>
       <c r="C46" t="s">
@@ -3451,15 +3476,15 @@
       <c r="H46" t="s">
         <v>36</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>172</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="6" t="s">
         <v>191</v>
       </c>
       <c r="C47" t="s">
@@ -3480,42 +3505,42 @@
       <c r="H47" t="s">
         <v>36</v>
       </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>193</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>194</v>
       </c>
       <c r="C48" t="s">
         <v>195</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="1">
         <v>39879</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" t="s">
         <v>129</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="3" t="s">
+      <c r="H48" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" t="s">
         <v>197</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J48" s="4">
         <v>51.5167</v>
       </c>
-      <c r="K48" s="6">
+      <c r="K48" s="4">
         <v>11.166700000000001</v>
       </c>
       <c r="M48" t="s">
@@ -3526,7 +3551,7 @@
       <c r="A49" t="s">
         <v>196</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>198</v>
       </c>
       <c r="C49" t="s">
@@ -3550,10 +3575,10 @@
       <c r="I49" t="s">
         <v>201</v>
       </c>
-      <c r="J49" s="6">
+      <c r="J49" s="4">
         <v>47.083329999999997</v>
       </c>
-      <c r="K49" s="6">
+      <c r="K49" s="4">
         <v>8</v>
       </c>
       <c r="M49" t="s">
@@ -3564,7 +3589,7 @@
       <c r="A50" t="s">
         <v>200</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>202</v>
       </c>
       <c r="C50" t="s">
@@ -3588,14 +3613,14 @@
       <c r="I50" t="s">
         <v>205</v>
       </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>204</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>206</v>
       </c>
       <c r="C51" t="s">
@@ -3619,14 +3644,14 @@
       <c r="I51" t="s">
         <v>209</v>
       </c>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>208</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>210</v>
       </c>
       <c r="C52" t="s">
@@ -3650,14 +3675,14 @@
       <c r="I52" t="s">
         <v>213</v>
       </c>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>212</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C53" t="s">
@@ -3681,14 +3706,14 @@
       <c r="I53" t="s">
         <v>217</v>
       </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>216</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>218</v>
       </c>
       <c r="C54" t="s">
@@ -3712,14 +3737,14 @@
       <c r="I54" t="s">
         <v>221</v>
       </c>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>220</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C55" t="s">
@@ -3743,14 +3768,14 @@
       <c r="I55" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>224</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>227</v>
       </c>
       <c r="C56" t="s">
@@ -3774,14 +3799,14 @@
       <c r="I56" t="s">
         <v>230</v>
       </c>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>229</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>231</v>
       </c>
       <c r="C57" t="s">
@@ -3805,14 +3830,14 @@
       <c r="I57" t="s">
         <v>234</v>
       </c>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>233</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>235</v>
       </c>
       <c r="C58" t="s">
@@ -3836,14 +3861,14 @@
       <c r="I58" t="s">
         <v>238</v>
       </c>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>33</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>239</v>
       </c>
       <c r="C59" t="s">
@@ -3867,14 +3892,14 @@
       <c r="I59" t="s">
         <v>242</v>
       </c>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>243</v>
       </c>
       <c r="C60" t="s">
@@ -3898,14 +3923,14 @@
       <c r="I60" t="s">
         <v>246</v>
       </c>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>187</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>247</v>
       </c>
       <c r="C61" t="s">
@@ -3929,21 +3954,21 @@
       <c r="I61" t="s">
         <v>250</v>
       </c>
-      <c r="J61" s="6">
+      <c r="J61" s="4">
         <v>47.145499999999998</v>
       </c>
-      <c r="K61" s="6">
+      <c r="K61" s="4">
         <v>17.622399999999999</v>
       </c>
       <c r="M61" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>190</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="6" t="s">
         <v>251</v>
       </c>
       <c r="C62" t="s">
@@ -3967,14 +3992,14 @@
       <c r="I62" t="s">
         <v>254</v>
       </c>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>237</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>255</v>
       </c>
       <c r="C63" t="s">
@@ -3998,14 +4023,14 @@
       <c r="I63" t="s">
         <v>230</v>
       </c>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>241</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>258</v>
       </c>
       <c r="C64" t="s">
@@ -4029,14 +4054,14 @@
       <c r="I64" t="s">
         <v>261</v>
       </c>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>245</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>262</v>
       </c>
       <c r="C65" t="s">
@@ -4060,14 +4085,14 @@
       <c r="I65" t="s">
         <v>264</v>
       </c>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>249</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C66" t="s">
@@ -4091,14 +4116,14 @@
       <c r="I66" t="s">
         <v>268</v>
       </c>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>134</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>269</v>
       </c>
       <c r="C67" t="s">
@@ -4122,14 +4147,14 @@
       <c r="I67" t="s">
         <v>272</v>
       </c>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>139</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>273</v>
       </c>
       <c r="C68" t="s">
@@ -4153,14 +4178,14 @@
       <c r="I68" t="s">
         <v>276</v>
       </c>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>144</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="5" t="s">
         <v>277</v>
       </c>
       <c r="C69" t="s">
@@ -4184,14 +4209,14 @@
       <c r="I69" t="s">
         <v>281</v>
       </c>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C70" t="s">
@@ -4215,14 +4240,14 @@
       <c r="I70" t="s">
         <v>284</v>
       </c>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>154</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>285</v>
       </c>
       <c r="C71" t="s">
@@ -4246,14 +4271,14 @@
       <c r="I71" t="s">
         <v>287</v>
       </c>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>157</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>288</v>
       </c>
       <c r="C72" t="s">
@@ -4277,14 +4302,14 @@
       <c r="I72" t="s">
         <v>287</v>
       </c>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>161</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>291</v>
       </c>
       <c r="C73" t="s">
@@ -4308,14 +4333,14 @@
       <c r="I73" t="s">
         <v>114</v>
       </c>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>165</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>294</v>
       </c>
       <c r="C74" t="s">
@@ -4339,14 +4364,14 @@
       <c r="I74" t="s">
         <v>296</v>
       </c>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>168</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>297</v>
       </c>
       <c r="C75" t="s">
@@ -4370,14 +4395,14 @@
       <c r="I75" t="s">
         <v>299</v>
       </c>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>171</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>300</v>
       </c>
       <c r="C76" t="s">
@@ -4401,14 +4426,14 @@
       <c r="I76" t="s">
         <v>221</v>
       </c>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>175</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>302</v>
       </c>
       <c r="C77" t="s">
@@ -4432,14 +4457,14 @@
       <c r="I77" t="s">
         <v>304</v>
       </c>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>178</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="5" t="s">
         <v>305</v>
       </c>
       <c r="C78" t="s">
@@ -4463,14 +4488,14 @@
       <c r="I78" t="s">
         <v>308</v>
       </c>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>253</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>309</v>
       </c>
       <c r="C79" t="s">
@@ -4494,14 +4519,14 @@
       <c r="I79" t="s">
         <v>311</v>
       </c>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>257</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>312</v>
       </c>
       <c r="C80" t="s">
@@ -4525,17 +4550,17 @@
       <c r="I80" t="s">
         <v>315</v>
       </c>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>181</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" t="s">
         <v>317</v>
       </c>
       <c r="D81" t="s">
@@ -4556,10 +4581,10 @@
       <c r="I81" t="s">
         <v>319</v>
       </c>
-      <c r="J81" s="6">
+      <c r="J81" s="4">
         <v>50.45</v>
       </c>
-      <c r="K81" s="6">
+      <c r="K81" s="4">
         <v>30.5</v>
       </c>
       <c r="M81" t="s">
@@ -4570,10 +4595,10 @@
       <c r="A82" t="s">
         <v>184</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" t="s">
         <v>321</v>
       </c>
       <c r="D82" t="s">
@@ -4594,10 +4619,10 @@
       <c r="I82" t="s">
         <v>323</v>
       </c>
-      <c r="J82" s="6">
+      <c r="J82" s="4">
         <v>45.1</v>
       </c>
-      <c r="K82" s="6">
+      <c r="K82" s="4">
         <v>0.7</v>
       </c>
       <c r="M82" t="s">
@@ -4608,7 +4633,7 @@
       <c r="A83" t="s">
         <v>324</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>325</v>
       </c>
       <c r="C83" t="s">
@@ -4632,14 +4657,14 @@
       <c r="I83" t="s">
         <v>328</v>
       </c>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>329</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>330</v>
       </c>
       <c r="C84" t="s">
@@ -4663,14 +4688,14 @@
       <c r="I84" t="s">
         <v>333</v>
       </c>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>334</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>335</v>
       </c>
       <c r="C85" t="s">
@@ -4694,14 +4719,14 @@
       <c r="I85" t="s">
         <v>338</v>
       </c>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>339</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>340</v>
       </c>
       <c r="C86" t="s">
@@ -4725,11 +4750,2580 @@
       <c r="I86" t="s">
         <v>114</v>
       </c>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319C9727-8CAD-EB48-9C33-DE79EC35C361}">
+  <dimension ref="A1:N75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" t="s">
+        <v>359</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>356</v>
+      </c>
+      <c r="L1" t="s">
+        <v>357</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>2016</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>360</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>2010</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>361</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="4">
+        <v>49.954439999999998</v>
+      </c>
+      <c r="L3" s="4">
+        <v>14.175829999999999</v>
+      </c>
+      <c r="N3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>2010</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>361</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="4">
+        <v>49.954439999999998</v>
+      </c>
+      <c r="L4" s="4">
+        <v>14.175829999999999</v>
+      </c>
+      <c r="N4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>2011</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>361</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="4">
+        <v>50.693460000000002</v>
+      </c>
+      <c r="L5" s="4">
+        <v>15.84652</v>
+      </c>
+      <c r="N5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>2011</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>361</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4">
+        <v>50.693460000000002</v>
+      </c>
+      <c r="L6" s="4">
+        <v>15.84652</v>
+      </c>
+      <c r="N6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>2015</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>2015</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>2013</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>2013</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>2013</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>2015</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13">
+        <v>2015</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>2012</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15">
+        <v>2013</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16">
+        <v>2012</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>2012</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18">
+        <v>2009</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19">
+        <v>2013</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20">
+        <v>2013</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21">
+        <v>2013</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22">
+        <v>2013</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23">
+        <v>2008</v>
+      </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24">
+        <v>2012</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="1">
+        <v>41011</v>
+      </c>
+      <c r="G25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" t="s">
+        <v>360</v>
+      </c>
+      <c r="J25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="1">
+        <v>41013</v>
+      </c>
+      <c r="G26" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" t="s">
+        <v>360</v>
+      </c>
+      <c r="J26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27">
+        <v>2008</v>
+      </c>
+      <c r="G27" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" t="s">
+        <v>360</v>
+      </c>
+      <c r="J27" t="s">
+        <v>124</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28">
+        <v>2008</v>
+      </c>
+      <c r="G28" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" t="s">
+        <v>360</v>
+      </c>
+      <c r="J28" t="s">
+        <v>130</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29">
+        <v>1960</v>
+      </c>
+      <c r="G29" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" t="s">
+        <v>360</v>
+      </c>
+      <c r="J29" t="s">
+        <v>135</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F30">
+        <v>2002</v>
+      </c>
+      <c r="G30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" t="s">
+        <v>360</v>
+      </c>
+      <c r="J30" t="s">
+        <v>140</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31">
+        <v>2008</v>
+      </c>
+      <c r="G31" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" t="s">
+        <v>360</v>
+      </c>
+      <c r="J31" t="s">
+        <v>145</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32">
+        <v>2008</v>
+      </c>
+      <c r="G32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" t="s">
+        <v>360</v>
+      </c>
+      <c r="J32" t="s">
+        <v>150</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33">
+        <v>2008</v>
+      </c>
+      <c r="G33" t="s">
+        <v>108</v>
+      </c>
+      <c r="H33" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" t="s">
+        <v>360</v>
+      </c>
+      <c r="J33" t="s">
+        <v>135</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34">
+        <v>2008</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>360</v>
+      </c>
+      <c r="J34" t="s">
+        <v>130</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="1">
+        <v>40073</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="1">
+        <v>40073</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="1">
+        <v>40073</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" t="s">
+        <v>36</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>190</v>
+      </c>
+      <c r="F38" s="1">
+        <v>40073</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>196</v>
+      </c>
+      <c r="F39" s="1">
+        <v>39879</v>
+      </c>
+      <c r="G39" t="s">
+        <v>129</v>
+      </c>
+      <c r="H39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I39" t="s">
+        <v>361</v>
+      </c>
+      <c r="J39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K39" s="4">
+        <v>51.5167</v>
+      </c>
+      <c r="L39" s="4">
+        <v>11.166700000000001</v>
+      </c>
+      <c r="N39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" s="1">
+        <v>39904</v>
+      </c>
+      <c r="G40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" t="s">
+        <v>361</v>
+      </c>
+      <c r="J40" t="s">
+        <v>201</v>
+      </c>
+      <c r="K40" s="4">
+        <v>47.083329999999997</v>
+      </c>
+      <c r="L40" s="4">
+        <v>8</v>
+      </c>
+      <c r="N40" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C41" t="s">
+        <v>203</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>204</v>
+      </c>
+      <c r="F41" s="1">
+        <v>39897</v>
+      </c>
+      <c r="G41" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" t="s">
+        <v>360</v>
+      </c>
+      <c r="J41" t="s">
+        <v>205</v>
+      </c>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" s="1">
+        <v>39990</v>
+      </c>
+      <c r="G42" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" t="s">
+        <v>360</v>
+      </c>
+      <c r="J42" t="s">
+        <v>209</v>
+      </c>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" t="s">
+        <v>211</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>212</v>
+      </c>
+      <c r="F43" s="1">
+        <v>39843</v>
+      </c>
+      <c r="G43" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>360</v>
+      </c>
+      <c r="J43" t="s">
+        <v>213</v>
+      </c>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>216</v>
+      </c>
+      <c r="F44" s="1">
+        <v>40248</v>
+      </c>
+      <c r="G44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H44" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" t="s">
+        <v>360</v>
+      </c>
+      <c r="J44" t="s">
+        <v>217</v>
+      </c>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" t="s">
+        <v>219</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
+        <v>220</v>
+      </c>
+      <c r="F45" s="1">
+        <v>40242</v>
+      </c>
+      <c r="G45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I45" t="s">
+        <v>360</v>
+      </c>
+      <c r="J45" t="s">
+        <v>221</v>
+      </c>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" t="s">
+        <v>224</v>
+      </c>
+      <c r="F46" s="1">
+        <v>39525</v>
+      </c>
+      <c r="G46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H46" t="s">
+        <v>36</v>
+      </c>
+      <c r="I46" t="s">
+        <v>360</v>
+      </c>
+      <c r="J46" t="s">
+        <v>226</v>
+      </c>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" t="s">
+        <v>228</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" t="s">
+        <v>229</v>
+      </c>
+      <c r="F47" s="1">
+        <v>39840</v>
+      </c>
+      <c r="G47" t="s">
+        <v>129</v>
+      </c>
+      <c r="H47" t="s">
+        <v>36</v>
+      </c>
+      <c r="I47" t="s">
+        <v>360</v>
+      </c>
+      <c r="J47" t="s">
+        <v>230</v>
+      </c>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C48" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" t="s">
+        <v>233</v>
+      </c>
+      <c r="F48" s="1">
+        <v>39875</v>
+      </c>
+      <c r="G48" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" t="s">
+        <v>360</v>
+      </c>
+      <c r="J48" t="s">
+        <v>234</v>
+      </c>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" t="s">
+        <v>236</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" t="s">
+        <v>237</v>
+      </c>
+      <c r="F49" s="1">
+        <v>39528</v>
+      </c>
+      <c r="G49" t="s">
+        <v>129</v>
+      </c>
+      <c r="H49" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" t="s">
+        <v>360</v>
+      </c>
+      <c r="J49" t="s">
+        <v>238</v>
+      </c>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" t="s">
+        <v>241</v>
+      </c>
+      <c r="F50">
+        <v>2015</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" t="s">
+        <v>360</v>
+      </c>
+      <c r="J50" t="s">
+        <v>242</v>
+      </c>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51" t="s">
+        <v>244</v>
+      </c>
+      <c r="D51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" t="s">
+        <v>245</v>
+      </c>
+      <c r="F51">
+        <v>2016</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" t="s">
+        <v>360</v>
+      </c>
+      <c r="J51" t="s">
+        <v>246</v>
+      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C52" t="s">
+        <v>248</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
+        <v>249</v>
+      </c>
+      <c r="F52" s="1">
+        <v>39901</v>
+      </c>
+      <c r="G52" t="s">
+        <v>129</v>
+      </c>
+      <c r="H52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I52" t="s">
+        <v>361</v>
+      </c>
+      <c r="J52" t="s">
+        <v>250</v>
+      </c>
+      <c r="K52" s="4">
+        <v>47.145499999999998</v>
+      </c>
+      <c r="L52" s="4">
+        <v>17.622399999999999</v>
+      </c>
+      <c r="N52" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C53" t="s">
+        <v>256</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>257</v>
+      </c>
+      <c r="F53" s="1">
+        <v>39539</v>
+      </c>
+      <c r="G53" t="s">
+        <v>129</v>
+      </c>
+      <c r="H53" t="s">
+        <v>36</v>
+      </c>
+      <c r="I53" t="s">
+        <v>360</v>
+      </c>
+      <c r="J53" t="s">
+        <v>230</v>
+      </c>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>241</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" t="s">
+        <v>260</v>
+      </c>
+      <c r="F54" s="1">
+        <v>40217</v>
+      </c>
+      <c r="G54" t="s">
+        <v>129</v>
+      </c>
+      <c r="H54" t="s">
+        <v>36</v>
+      </c>
+      <c r="I54" t="s">
+        <v>360</v>
+      </c>
+      <c r="J54" t="s">
+        <v>261</v>
+      </c>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>245</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C55" t="s">
+        <v>263</v>
+      </c>
+      <c r="D55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="1">
+        <v>40242</v>
+      </c>
+      <c r="G55" t="s">
+        <v>129</v>
+      </c>
+      <c r="H55" t="s">
+        <v>36</v>
+      </c>
+      <c r="I55" t="s">
+        <v>360</v>
+      </c>
+      <c r="J55" t="s">
+        <v>264</v>
+      </c>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C56" t="s">
+        <v>266</v>
+      </c>
+      <c r="D56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56" t="s">
+        <v>267</v>
+      </c>
+      <c r="F56" s="1">
+        <v>39882</v>
+      </c>
+      <c r="G56" t="s">
+        <v>225</v>
+      </c>
+      <c r="H56" t="s">
+        <v>36</v>
+      </c>
+      <c r="I56" t="s">
+        <v>360</v>
+      </c>
+      <c r="J56" t="s">
+        <v>268</v>
+      </c>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" s="1">
+        <v>40205</v>
+      </c>
+      <c r="G57" t="s">
+        <v>129</v>
+      </c>
+      <c r="H57" t="s">
+        <v>36</v>
+      </c>
+      <c r="I57" t="s">
+        <v>360</v>
+      </c>
+      <c r="J57" t="s">
+        <v>272</v>
+      </c>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" t="s">
+        <v>274</v>
+      </c>
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58" t="s">
+        <v>275</v>
+      </c>
+      <c r="F58" s="1">
+        <v>40252</v>
+      </c>
+      <c r="G58" t="s">
+        <v>129</v>
+      </c>
+      <c r="H58" t="s">
+        <v>36</v>
+      </c>
+      <c r="I58" t="s">
+        <v>360</v>
+      </c>
+      <c r="J58" t="s">
+        <v>276</v>
+      </c>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C59" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E59" t="s">
+        <v>280</v>
+      </c>
+      <c r="F59" s="1">
+        <v>40275</v>
+      </c>
+      <c r="G59" t="s">
+        <v>129</v>
+      </c>
+      <c r="H59" t="s">
+        <v>36</v>
+      </c>
+      <c r="I59" t="s">
+        <v>360</v>
+      </c>
+      <c r="J59" t="s">
+        <v>281</v>
+      </c>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" t="s">
+        <v>286</v>
+      </c>
+      <c r="D60" t="s">
+        <v>279</v>
+      </c>
+      <c r="E60" t="s">
+        <v>280</v>
+      </c>
+      <c r="F60">
+        <v>2016</v>
+      </c>
+      <c r="G60" t="s">
+        <v>34</v>
+      </c>
+      <c r="H60" t="s">
+        <v>36</v>
+      </c>
+      <c r="I60" t="s">
+        <v>362</v>
+      </c>
+      <c r="J60" t="s">
+        <v>287</v>
+      </c>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C61" t="s">
+        <v>289</v>
+      </c>
+      <c r="D61" t="s">
+        <v>279</v>
+      </c>
+      <c r="E61" t="s">
+        <v>290</v>
+      </c>
+      <c r="F61">
+        <v>2016</v>
+      </c>
+      <c r="G61" t="s">
+        <v>34</v>
+      </c>
+      <c r="H61" t="s">
+        <v>36</v>
+      </c>
+      <c r="I61" t="s">
+        <v>362</v>
+      </c>
+      <c r="J61" t="s">
+        <v>287</v>
+      </c>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>161</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C62" t="s">
+        <v>292</v>
+      </c>
+      <c r="D62" t="s">
+        <v>279</v>
+      </c>
+      <c r="E62" t="s">
+        <v>293</v>
+      </c>
+      <c r="F62" s="1">
+        <v>41011</v>
+      </c>
+      <c r="G62" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" t="s">
+        <v>36</v>
+      </c>
+      <c r="I62" t="s">
+        <v>360</v>
+      </c>
+      <c r="J62" t="s">
+        <v>114</v>
+      </c>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C63" t="s">
+        <v>295</v>
+      </c>
+      <c r="D63" t="s">
+        <v>279</v>
+      </c>
+      <c r="E63" t="s">
+        <v>280</v>
+      </c>
+      <c r="F63" s="1">
+        <v>40987</v>
+      </c>
+      <c r="G63" t="s">
+        <v>108</v>
+      </c>
+      <c r="H63" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" t="s">
+        <v>360</v>
+      </c>
+      <c r="J63" t="s">
+        <v>296</v>
+      </c>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" t="s">
+        <v>279</v>
+      </c>
+      <c r="E64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F64" s="1">
+        <v>40590</v>
+      </c>
+      <c r="G64" t="s">
+        <v>129</v>
+      </c>
+      <c r="H64" t="s">
+        <v>36</v>
+      </c>
+      <c r="I64" t="s">
+        <v>360</v>
+      </c>
+      <c r="J64" t="s">
+        <v>299</v>
+      </c>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C65" t="s">
+        <v>301</v>
+      </c>
+      <c r="D65" t="s">
+        <v>279</v>
+      </c>
+      <c r="E65" t="s">
+        <v>290</v>
+      </c>
+      <c r="F65" s="1">
+        <v>40583</v>
+      </c>
+      <c r="G65" t="s">
+        <v>129</v>
+      </c>
+      <c r="H65" t="s">
+        <v>36</v>
+      </c>
+      <c r="I65" t="s">
+        <v>360</v>
+      </c>
+      <c r="J65" t="s">
+        <v>221</v>
+      </c>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C66" t="s">
+        <v>303</v>
+      </c>
+      <c r="D66" t="s">
+        <v>279</v>
+      </c>
+      <c r="E66" t="s">
+        <v>293</v>
+      </c>
+      <c r="F66" s="1">
+        <v>40572</v>
+      </c>
+      <c r="G66" t="s">
+        <v>129</v>
+      </c>
+      <c r="H66" t="s">
+        <v>36</v>
+      </c>
+      <c r="I66" t="s">
+        <v>360</v>
+      </c>
+      <c r="J66" t="s">
+        <v>304</v>
+      </c>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>178</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C67" t="s">
+        <v>306</v>
+      </c>
+      <c r="D67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E67" t="s">
+        <v>307</v>
+      </c>
+      <c r="F67" s="1">
+        <v>40566</v>
+      </c>
+      <c r="G67" t="s">
+        <v>225</v>
+      </c>
+      <c r="H67" t="s">
+        <v>36</v>
+      </c>
+      <c r="I67" t="s">
+        <v>360</v>
+      </c>
+      <c r="J67" t="s">
+        <v>308</v>
+      </c>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>253</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C68" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" t="s">
+        <v>279</v>
+      </c>
+      <c r="E68" t="s">
+        <v>307</v>
+      </c>
+      <c r="F68" s="1">
+        <v>40969</v>
+      </c>
+      <c r="G68" t="s">
+        <v>108</v>
+      </c>
+      <c r="H68" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" t="s">
+        <v>360</v>
+      </c>
+      <c r="J68" t="s">
+        <v>311</v>
+      </c>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>257</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C69" t="s">
+        <v>313</v>
+      </c>
+      <c r="D69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" t="s">
+        <v>314</v>
+      </c>
+      <c r="F69" s="1">
+        <v>40889</v>
+      </c>
+      <c r="G69" t="s">
+        <v>108</v>
+      </c>
+      <c r="H69" t="s">
+        <v>36</v>
+      </c>
+      <c r="I69" t="s">
+        <v>360</v>
+      </c>
+      <c r="J69" t="s">
+        <v>315</v>
+      </c>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C70" t="s">
+        <v>317</v>
+      </c>
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>318</v>
+      </c>
+      <c r="F70" s="1">
+        <v>40577</v>
+      </c>
+      <c r="G70" t="s">
+        <v>108</v>
+      </c>
+      <c r="H70" t="s">
+        <v>36</v>
+      </c>
+      <c r="I70" t="s">
+        <v>361</v>
+      </c>
+      <c r="J70" t="s">
+        <v>319</v>
+      </c>
+      <c r="K70" s="4">
+        <v>50.45</v>
+      </c>
+      <c r="L70" s="4">
+        <v>30.5</v>
+      </c>
+      <c r="N70" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C71" t="s">
+        <v>321</v>
+      </c>
+      <c r="D71" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" t="s">
+        <v>322</v>
+      </c>
+      <c r="F71" s="1">
+        <v>39884</v>
+      </c>
+      <c r="G71" t="s">
+        <v>108</v>
+      </c>
+      <c r="H71" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" t="s">
+        <v>361</v>
+      </c>
+      <c r="J71" t="s">
+        <v>323</v>
+      </c>
+      <c r="K71" s="4">
+        <v>45.1</v>
+      </c>
+      <c r="L71" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="N71" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>324</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C72" t="s">
+        <v>326</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>327</v>
+      </c>
+      <c r="F72">
+        <v>2014</v>
+      </c>
+      <c r="G72" t="s">
+        <v>108</v>
+      </c>
+      <c r="H72" t="s">
+        <v>36</v>
+      </c>
+      <c r="I72" t="s">
+        <v>360</v>
+      </c>
+      <c r="J72" t="s">
+        <v>328</v>
+      </c>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C73" t="s">
+        <v>331</v>
+      </c>
+      <c r="D73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E73" t="s">
+        <v>332</v>
+      </c>
+      <c r="F73">
+        <v>2013</v>
+      </c>
+      <c r="G73" t="s">
+        <v>108</v>
+      </c>
+      <c r="H73" t="s">
+        <v>36</v>
+      </c>
+      <c r="I73" t="s">
+        <v>360</v>
+      </c>
+      <c r="J73" t="s">
+        <v>333</v>
+      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>334</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C74" t="s">
+        <v>336</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>337</v>
+      </c>
+      <c r="F74" s="1">
+        <v>40967</v>
+      </c>
+      <c r="G74" t="s">
+        <v>108</v>
+      </c>
+      <c r="H74" t="s">
+        <v>36</v>
+      </c>
+      <c r="I74" t="s">
+        <v>360</v>
+      </c>
+      <c r="J74" t="s">
+        <v>338</v>
+      </c>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>339</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C75" t="s">
+        <v>341</v>
+      </c>
+      <c r="D75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E75" t="s">
+        <v>342</v>
+      </c>
+      <c r="F75">
+        <v>2012</v>
+      </c>
+      <c r="G75" t="s">
+        <v>108</v>
+      </c>
+      <c r="H75" t="s">
+        <v>36</v>
+      </c>
+      <c r="I75" t="s">
+        <v>360</v>
+      </c>
+      <c r="J75" t="s">
+        <v>114</v>
+      </c>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>